<commit_message>
26/04/2021 - Arreglando bugs
</commit_message>
<xml_diff>
--- a/reports/productos/productos.xlsx
+++ b/reports/productos/productos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Fecha de creación</t>
   </si>
@@ -56,21 +56,6 @@
   </si>
   <si>
     <t>Activo</t>
-  </si>
-  <si>
-    <t>LB0002</t>
-  </si>
-  <si>
-    <t>ZAPATOS</t>
-  </si>
-  <si>
-    <t>UNIDAD</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Inactivo</t>
   </si>
 </sst>
 </file>
@@ -451,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -520,35 +505,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>1500.67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3">
-        <v>180</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
02/05/2021 - Guia de usuario
</commit_message>
<xml_diff>
--- a/reports/productos/productos.xlsx
+++ b/reports/productos/productos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Fecha de creación</t>
   </si>
@@ -37,7 +37,7 @@
     <t>¿Cantidad minima?</t>
   </si>
   <si>
-    <t>estado</t>
+    <t>Estado</t>
   </si>
   <si>
     <t>18/04/2021</t>
@@ -56,6 +56,27 @@
   </si>
   <si>
     <t>Activo</t>
+  </si>
+  <si>
+    <t>27/04/2021</t>
+  </si>
+  <si>
+    <t>LB0003</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>LB0002</t>
+  </si>
+  <si>
+    <t>ZAPATOS</t>
+  </si>
+  <si>
+    <t>UNIDAD</t>
+  </si>
+  <si>
+    <t>Inactivo</t>
   </si>
 </sst>
 </file>
@@ -436,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -487,13 +508,13 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>1200</v>
+        <v>1200.5446543232</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -503,6 +524,64 @@
       </c>
       <c r="I2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>1500.67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>180</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>